<commit_message>
update more exam and explain
</commit_message>
<xml_diff>
--- a/NOTE_OCA.xlsx
+++ b/NOTE_OCA.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8701" uniqueCount="3686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8712" uniqueCount="3686">
   <si>
     <t>1.1 Comments:</t>
   </si>
@@ -17575,11 +17575,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -22055,16 +22055,16 @@
       <c r="C562" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D562" s="306" t="s">
+      <c r="D562" s="307" t="s">
         <v>219</v>
       </c>
-      <c r="E562" s="306"/>
-      <c r="F562" s="306"/>
-      <c r="G562" s="306"/>
-      <c r="H562" s="306"/>
-      <c r="I562" s="306"/>
-      <c r="J562" s="306"/>
-      <c r="K562" s="306"/>
+      <c r="E562" s="307"/>
+      <c r="F562" s="307"/>
+      <c r="G562" s="307"/>
+      <c r="H562" s="307"/>
+      <c r="I562" s="307"/>
+      <c r="J562" s="307"/>
+      <c r="K562" s="307"/>
       <c r="L562" s="3" t="s">
         <v>89</v>
       </c>
@@ -22131,16 +22131,16 @@
       <c r="C568" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D568" s="306" t="s">
+      <c r="D568" s="307" t="s">
         <v>232</v>
       </c>
-      <c r="E568" s="306"/>
-      <c r="F568" s="306"/>
-      <c r="G568" s="306"/>
-      <c r="H568" s="306"/>
-      <c r="I568" s="306"/>
-      <c r="J568" s="306"/>
-      <c r="K568" s="306"/>
+      <c r="E568" s="307"/>
+      <c r="F568" s="307"/>
+      <c r="G568" s="307"/>
+      <c r="H568" s="307"/>
+      <c r="I568" s="307"/>
+      <c r="J568" s="307"/>
+      <c r="K568" s="307"/>
       <c r="L568" s="3" t="s">
         <v>41</v>
       </c>
@@ -23626,8 +23626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A388" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E402" sqref="E402"/>
+    <sheetView tabSelected="1" topLeftCell="A397" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D408" sqref="D408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27458,7 +27458,7 @@
       <c r="D360" s="70" t="s">
         <v>623</v>
       </c>
-      <c r="G360" s="307" t="s">
+      <c r="G360" s="306" t="s">
         <v>3659</v>
       </c>
       <c r="H360" s="43"/>
@@ -27479,7 +27479,7 @@
       <c r="D361" s="288" t="s">
         <v>208</v>
       </c>
-      <c r="G361" s="307" t="s">
+      <c r="G361" s="306" t="s">
         <v>3660</v>
       </c>
       <c r="H361" s="43"/>
@@ -27500,7 +27500,7 @@
       <c r="D362" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="G362" s="307" t="s">
+      <c r="G362" s="306" t="s">
         <v>605</v>
       </c>
       <c r="H362" s="43"/>
@@ -27519,7 +27519,7 @@
       <c r="D363" s="288" t="s">
         <v>210</v>
       </c>
-      <c r="G363" s="307" t="s">
+      <c r="G363" s="306" t="s">
         <v>37</v>
       </c>
       <c r="H363" s="43"/>
@@ -27552,7 +27552,7 @@
       <c r="F365" t="s">
         <v>3683</v>
       </c>
-      <c r="G365" s="307" t="s">
+      <c r="G365" s="306" t="s">
         <v>3684</v>
       </c>
     </row>
@@ -27895,77 +27895,99 @@
       <c r="B404" s="67">
         <v>26</v>
       </c>
-      <c r="C404" s="67"/>
+      <c r="C404" s="292" t="s">
+        <v>209</v>
+      </c>
       <c r="D404" s="67"/>
     </row>
     <row r="405" spans="2:4">
       <c r="B405" s="67">
         <v>27</v>
       </c>
-      <c r="C405" s="67"/>
+      <c r="C405" s="67" t="s">
+        <v>210</v>
+      </c>
       <c r="D405" s="67"/>
     </row>
     <row r="406" spans="2:4">
       <c r="B406" s="67">
         <v>28</v>
       </c>
-      <c r="C406" s="67"/>
+      <c r="C406" s="67" t="s">
+        <v>673</v>
+      </c>
       <c r="D406" s="67"/>
     </row>
     <row r="407" spans="2:4">
       <c r="B407" s="67">
         <v>29</v>
       </c>
-      <c r="C407" s="67"/>
+      <c r="C407" s="67" t="s">
+        <v>201</v>
+      </c>
       <c r="D407" s="67"/>
     </row>
     <row r="408" spans="2:4">
       <c r="B408" s="67">
         <v>30</v>
       </c>
-      <c r="C408" s="67"/>
+      <c r="C408" s="67" t="s">
+        <v>245</v>
+      </c>
       <c r="D408" s="67"/>
     </row>
     <row r="409" spans="2:4">
       <c r="B409" s="67">
         <v>31</v>
       </c>
-      <c r="C409" s="67"/>
+      <c r="C409" s="67" t="s">
+        <v>204</v>
+      </c>
       <c r="D409" s="67"/>
     </row>
     <row r="410" spans="2:4">
       <c r="B410" s="67">
         <v>32</v>
       </c>
-      <c r="C410" s="67"/>
+      <c r="C410" s="67" t="s">
+        <v>204</v>
+      </c>
       <c r="D410" s="67"/>
     </row>
     <row r="411" spans="2:4">
       <c r="B411" s="67">
         <v>33</v>
       </c>
-      <c r="C411" s="67"/>
+      <c r="C411" s="67" t="s">
+        <v>210</v>
+      </c>
       <c r="D411" s="67"/>
     </row>
     <row r="412" spans="2:4">
       <c r="B412" s="67">
         <v>34</v>
       </c>
-      <c r="C412" s="67"/>
+      <c r="C412" s="67" t="s">
+        <v>201</v>
+      </c>
       <c r="D412" s="67"/>
     </row>
     <row r="413" spans="2:4">
       <c r="B413" s="67">
         <v>35</v>
       </c>
-      <c r="C413" s="67"/>
+      <c r="C413" s="292" t="s">
+        <v>203</v>
+      </c>
       <c r="D413" s="67"/>
     </row>
     <row r="414" spans="2:4">
       <c r="B414" s="67">
         <v>36</v>
       </c>
-      <c r="C414" s="67"/>
+      <c r="C414" s="67" t="s">
+        <v>245</v>
+      </c>
       <c r="D414" s="67"/>
     </row>
     <row r="415" spans="2:4">

</xml_diff>